<commit_message>
update data extraction 20230709
</commit_message>
<xml_diff>
--- a/master_data/categories.xlsx
+++ b/master_data/categories.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72f513831c36f08e/Trabajos/jobs-data-cleaning/master_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{2877C737-C43A-48A3-BDB4-0BE7D5B98A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93EA33A1-038D-490E-837C-F8A61B145C32}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="8_{2877C737-C43A-48A3-BDB4-0BE7D5B98A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1424C341-13AB-4AA3-8D59-F86C363219FA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C6B871D3-577A-4CAC-9580-1E4AECA8D0D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$63</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="76">
   <si>
     <t>data scientist</t>
   </si>
@@ -47,12 +50,6 @@
     <t>machine learning</t>
   </si>
   <si>
-    <t xml:space="preserve">ds </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ml </t>
-  </si>
-  <si>
     <t>artificial</t>
   </si>
   <si>
@@ -258,6 +255,18 @@
   </si>
   <si>
     <t>market</t>
+  </si>
+  <si>
+    <t>-bi</t>
+  </si>
+  <si>
+    <t>Tableau</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ds </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ml </t>
   </si>
 </sst>
 </file>
@@ -293,8 +302,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C26501AA-1886-4A42-8E7C-EA0B04F49929}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,18 +634,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -643,7 +653,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -651,15 +661,15 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,375 +677,375 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B42" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -1048,23 +1058,23 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>34</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
@@ -1072,45 +1082,62 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B59" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>33</v>
-      </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B63" xr:uid="{C26501AA-1886-4A42-8E7C-EA0B04F49929}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>